<commit_message>
Notes, update bom_compare.xlsx for input board build.
</commit_message>
<xml_diff>
--- a/parts/bom_compare.xlsx
+++ b/parts/bom_compare.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robma\Documents\Work\ilemt_hw\parts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B83D144-F309-42B4-A71D-AA0FD3982D98}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{18A8EB58-7F7C-4298-B103-9ACD5A4DBC45}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9072" yWindow="792" windowWidth="28308" windowHeight="24912" tabRatio="500" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="1992" windowHeight="564" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="help" sheetId="3" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="kicad_bom" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1611" uniqueCount="659">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1615" uniqueCount="665">
   <si>
     <t>Index</t>
   </si>
@@ -2010,6 +2011,24 @@
   </si>
   <si>
     <t>Num assemblies:</t>
+  </si>
+  <si>
+    <t>490-GCM2195C1K103FA16DCT-ND</t>
+  </si>
+  <si>
+    <t>GCM2195C1K103FA16D</t>
+  </si>
+  <si>
+    <t>CERAMIC CAP AEC-Q200</t>
+  </si>
+  <si>
+    <t>YAG1859CT-ND</t>
+  </si>
+  <si>
+    <t>RT0805BRD072KL</t>
+  </si>
+  <si>
+    <t>RES SMD 2K OHM 0.1% 1/8W 0805</t>
   </si>
 </sst>
 </file>
@@ -2122,7 +2141,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2178,6 +2197,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2187,8 +2209,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2573,180 +2593,180 @@
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:11" ht="14.4" customHeight="1">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="30" t="s">
         <v>630</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="27"/>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="27"/>
-      <c r="J3" s="27"/>
-      <c r="K3" s="27"/>
+      <c r="A3" s="30"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
     </row>
     <row r="4" spans="1:11" s="5" customFormat="1">
-      <c r="A4" s="27"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
-      <c r="K4" s="27"/>
+      <c r="A4" s="30"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
     </row>
     <row r="5" spans="1:11" s="5" customFormat="1">
-      <c r="A5" s="27"/>
-      <c r="B5" s="27"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="27"/>
-      <c r="J5" s="27"/>
-      <c r="K5" s="27"/>
+      <c r="A5" s="30"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="30"/>
+      <c r="K5" s="30"/>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="27"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
-      <c r="I6" s="27"/>
-      <c r="J6" s="27"/>
-      <c r="K6" s="27"/>
+      <c r="A6" s="30"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="30"/>
     </row>
     <row r="7" spans="1:11" s="5" customFormat="1" ht="14.4" customHeight="1">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="32" t="s">
         <v>629</v>
       </c>
-      <c r="B7" s="29"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
-      <c r="H7" s="29"/>
-      <c r="I7" s="29"/>
-      <c r="J7" s="29"/>
-      <c r="K7" s="29"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="32"/>
+      <c r="K7" s="32"/>
     </row>
     <row r="8" spans="1:11" s="5" customFormat="1" ht="14.4" customHeight="1">
-      <c r="A8" s="29"/>
-      <c r="B8" s="29"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="29"/>
-      <c r="K8" s="29"/>
+      <c r="A8" s="32"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="32"/>
+      <c r="J8" s="32"/>
+      <c r="K8" s="32"/>
     </row>
     <row r="9" spans="1:11" s="5" customFormat="1">
-      <c r="A9" s="29"/>
-      <c r="B9" s="29"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="29"/>
-      <c r="I9" s="29"/>
-      <c r="J9" s="29"/>
-      <c r="K9" s="29"/>
+      <c r="A9" s="32"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="32"/>
     </row>
     <row r="10" spans="1:11" s="5" customFormat="1"/>
     <row r="11" spans="1:11" s="5" customFormat="1">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="31" t="s">
         <v>628</v>
       </c>
-      <c r="B11" s="28"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="28"/>
-      <c r="K11" s="28"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="31"/>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="28"/>
-      <c r="B12" s="28"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="28"/>
-      <c r="I12" s="28"/>
-      <c r="J12" s="28"/>
-      <c r="K12" s="28"/>
+      <c r="A12" s="31"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="31"/>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="28"/>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="28"/>
-      <c r="K13" s="28"/>
+      <c r="A13" s="31"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="31"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="31"/>
     </row>
     <row r="14" spans="1:11">
-      <c r="A14" s="28"/>
-      <c r="B14" s="28"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="28"/>
-      <c r="J14" s="28"/>
-      <c r="K14" s="28"/>
+      <c r="A14" s="31"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="31"/>
+      <c r="K14" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2760,10 +2780,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M63"/>
+  <dimension ref="A1:M64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M37" sqref="M37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O40" sqref="O40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2822,1966 +2842,2005 @@
       </c>
     </row>
     <row r="2" spans="1:13" s="2" customFormat="1">
-      <c r="A2" s="30">
-        <v>1</v>
-      </c>
-      <c r="B2" s="30">
+      <c r="A2" s="28">
+        <v>1</v>
+      </c>
+      <c r="B2" s="28">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="27" t="s">
         <v>633</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="27" t="s">
         <v>634</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="27" t="s">
         <v>635</v>
       </c>
-      <c r="G2" s="30">
+      <c r="F2" s="27"/>
+      <c r="G2" s="28">
         <v>4</v>
       </c>
-      <c r="H2" s="30">
-        <v>0</v>
-      </c>
-      <c r="I2" s="2">
+      <c r="H2" s="28">
+        <v>0</v>
+      </c>
+      <c r="I2" s="27">
         <v>11.62</v>
       </c>
-      <c r="J2" s="31">
+      <c r="J2" s="29">
         <v>46.48</v>
       </c>
     </row>
     <row r="3" spans="1:13" s="2" customFormat="1">
-      <c r="A3" s="30">
+      <c r="A3" s="28">
         <v>2</v>
       </c>
-      <c r="B3" s="30">
+      <c r="B3" s="28">
         <v>4</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="27" t="s">
         <v>636</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="27" t="s">
         <v>637</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="27" t="s">
         <v>638</v>
       </c>
-      <c r="G3" s="30">
+      <c r="F3" s="27"/>
+      <c r="G3" s="28">
         <v>4</v>
       </c>
-      <c r="H3" s="30">
-        <v>0</v>
-      </c>
-      <c r="I3" s="2">
+      <c r="H3" s="28">
+        <v>0</v>
+      </c>
+      <c r="I3" s="27">
         <v>19.059999999999999</v>
       </c>
-      <c r="J3" s="31">
+      <c r="J3" s="29">
         <v>76.239999999999995</v>
       </c>
     </row>
     <row r="4" spans="1:13" s="2" customFormat="1">
-      <c r="A4" s="30">
+      <c r="A4" s="28">
         <v>3</v>
       </c>
-      <c r="B4" s="30">
+      <c r="B4" s="28">
         <v>20</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="27" t="s">
         <v>181</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="27" t="s">
         <v>182</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="27" t="s">
         <v>180</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="27" t="s">
         <v>179</v>
       </c>
-      <c r="G4" s="30">
+      <c r="G4" s="28">
         <v>20</v>
       </c>
-      <c r="H4" s="30">
-        <v>0</v>
-      </c>
-      <c r="I4" s="2">
+      <c r="H4" s="28">
+        <v>0</v>
+      </c>
+      <c r="I4" s="27">
         <v>0.21299999999999999</v>
       </c>
-      <c r="J4" s="31">
+      <c r="J4" s="29">
         <v>4.26</v>
       </c>
     </row>
     <row r="5" spans="1:13" s="2" customFormat="1">
-      <c r="A5" s="30">
+      <c r="A5" s="28">
         <v>4</v>
       </c>
-      <c r="B5" s="30">
+      <c r="B5" s="28">
         <v>6</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="27" t="s">
         <v>484</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="27" t="s">
         <v>485</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="27" t="s">
         <v>483</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="27" t="s">
         <v>482</v>
       </c>
-      <c r="G5" s="30">
+      <c r="G5" s="28">
         <v>6</v>
       </c>
-      <c r="H5" s="30">
-        <v>0</v>
-      </c>
-      <c r="I5" s="2">
+      <c r="H5" s="28">
+        <v>0</v>
+      </c>
+      <c r="I5" s="27">
         <v>21.04</v>
       </c>
-      <c r="J5" s="31">
+      <c r="J5" s="29">
         <v>126.24</v>
       </c>
     </row>
     <row r="6" spans="1:13" s="2" customFormat="1">
-      <c r="A6" s="30">
+      <c r="A6" s="28">
         <v>5</v>
       </c>
-      <c r="B6" s="30">
+      <c r="B6" s="28">
         <v>10</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="27" t="s">
         <v>265</v>
       </c>
-      <c r="G6" s="30">
+      <c r="G6" s="28">
         <v>10</v>
       </c>
-      <c r="H6" s="30">
-        <v>0</v>
-      </c>
-      <c r="I6" s="2">
+      <c r="H6" s="28">
+        <v>0</v>
+      </c>
+      <c r="I6" s="27">
         <v>0.151</v>
       </c>
-      <c r="J6" s="31">
+      <c r="J6" s="29">
         <v>1.51</v>
       </c>
     </row>
     <row r="7" spans="1:13" s="2" customFormat="1">
-      <c r="A7" s="30">
+      <c r="A7" s="28">
         <v>6</v>
       </c>
-      <c r="B7" s="30">
+      <c r="B7" s="28">
         <v>10</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="27" t="s">
         <v>417</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="27" t="s">
         <v>418</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="27" t="s">
         <v>416</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="27" t="s">
         <v>415</v>
       </c>
-      <c r="G7" s="30">
+      <c r="G7" s="28">
         <v>10</v>
       </c>
-      <c r="H7" s="30">
-        <v>0</v>
-      </c>
-      <c r="I7" s="2">
+      <c r="H7" s="28">
+        <v>0</v>
+      </c>
+      <c r="I7" s="27">
         <v>0.36099999999999999</v>
       </c>
-      <c r="J7" s="31">
+      <c r="J7" s="29">
         <v>3.61</v>
       </c>
     </row>
     <row r="8" spans="1:13" s="2" customFormat="1">
-      <c r="A8" s="30">
+      <c r="A8" s="28">
         <v>7</v>
       </c>
-      <c r="B8" s="30">
+      <c r="B8" s="28">
         <v>10</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="27" t="s">
         <v>523</v>
       </c>
-      <c r="G8" s="30">
+      <c r="G8" s="28">
         <v>10</v>
       </c>
-      <c r="H8" s="30">
-        <v>0</v>
-      </c>
-      <c r="I8" s="2">
+      <c r="H8" s="28">
+        <v>0</v>
+      </c>
+      <c r="I8" s="27">
         <v>0.47699999999999998</v>
       </c>
-      <c r="J8" s="31">
+      <c r="J8" s="29">
         <v>4.7699999999999996</v>
       </c>
     </row>
     <row r="9" spans="1:13" s="2" customFormat="1">
-      <c r="A9" s="30">
+      <c r="A9" s="28">
         <v>8</v>
       </c>
-      <c r="B9" s="30">
+      <c r="B9" s="28">
         <v>10</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="27" t="s">
         <v>476</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="27" t="s">
         <v>477</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="27" t="s">
         <v>475</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="27" t="s">
         <v>474</v>
       </c>
-      <c r="G9" s="30">
+      <c r="G9" s="28">
         <v>10</v>
       </c>
-      <c r="H9" s="30">
-        <v>0</v>
-      </c>
-      <c r="I9" s="2">
+      <c r="H9" s="28">
+        <v>0</v>
+      </c>
+      <c r="I9" s="27">
         <v>7.84</v>
       </c>
-      <c r="J9" s="31">
+      <c r="J9" s="29">
         <v>78.400000000000006</v>
       </c>
     </row>
     <row r="10" spans="1:13" s="2" customFormat="1">
-      <c r="A10" s="30">
+      <c r="A10" s="28">
         <v>9</v>
       </c>
-      <c r="B10" s="30">
+      <c r="B10" s="28">
         <v>10</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="27" t="s">
         <v>552</v>
       </c>
-      <c r="G10" s="30">
+      <c r="G10" s="28">
         <v>10</v>
       </c>
-      <c r="H10" s="30">
-        <v>0</v>
-      </c>
-      <c r="I10" s="2">
+      <c r="H10" s="28">
+        <v>0</v>
+      </c>
+      <c r="I10" s="27">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="J10" s="31">
+      <c r="J10" s="29">
         <v>0.65</v>
       </c>
     </row>
     <row r="11" spans="1:13" s="2" customFormat="1">
-      <c r="A11" s="30">
+      <c r="A11" s="28">
         <v>10</v>
       </c>
-      <c r="B11" s="30">
+      <c r="B11" s="28">
         <v>10</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="27" t="s">
         <v>407</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="27" t="s">
         <v>408</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="27" t="s">
         <v>557</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="27" t="s">
         <v>405</v>
       </c>
-      <c r="G11" s="30">
+      <c r="G11" s="28">
         <v>10</v>
       </c>
-      <c r="H11" s="30">
-        <v>0</v>
-      </c>
-      <c r="I11" s="2">
+      <c r="H11" s="28">
+        <v>0</v>
+      </c>
+      <c r="I11" s="27">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="J11" s="31">
+      <c r="J11" s="29">
         <v>0.48</v>
       </c>
     </row>
     <row r="12" spans="1:13" s="2" customFormat="1">
-      <c r="A12" s="30">
+      <c r="A12" s="28">
         <v>11</v>
       </c>
-      <c r="B12" s="30">
+      <c r="B12" s="28">
+        <v>3</v>
+      </c>
+      <c r="C12" s="27" t="s">
+        <v>276</v>
+      </c>
+      <c r="D12" s="27" t="s">
+        <v>277</v>
+      </c>
+      <c r="E12" s="27" t="s">
+        <v>275</v>
+      </c>
+      <c r="F12" s="27" t="s">
+        <v>274</v>
+      </c>
+      <c r="G12" s="28">
+        <v>3</v>
+      </c>
+      <c r="H12" s="28">
+        <v>0</v>
+      </c>
+      <c r="I12" s="27">
+        <v>1.66</v>
+      </c>
+      <c r="J12" s="29">
+        <v>4.9800000000000004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" s="2" customFormat="1">
+      <c r="A13" s="28">
+        <v>12</v>
+      </c>
+      <c r="B13" s="28">
+        <v>50</v>
+      </c>
+      <c r="C13" s="27" t="s">
+        <v>559</v>
+      </c>
+      <c r="D13" s="27" t="s">
+        <v>558</v>
+      </c>
+      <c r="E13" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="27" t="s">
+        <v>218</v>
+      </c>
+      <c r="G13" s="28">
+        <v>50</v>
+      </c>
+      <c r="H13" s="28">
+        <v>0</v>
+      </c>
+      <c r="I13" s="27">
+        <v>0.72460000000000002</v>
+      </c>
+      <c r="J13" s="29">
+        <v>36.229999999999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" s="2" customFormat="1">
+      <c r="A14" s="28">
+        <v>13</v>
+      </c>
+      <c r="B14" s="28">
         <v>10</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>396</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>397</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="F12" s="2" t="s">
+      <c r="C14" s="27" t="s">
+        <v>517</v>
+      </c>
+      <c r="D14" s="27" t="s">
+        <v>518</v>
+      </c>
+      <c r="E14" s="27" t="s">
+        <v>516</v>
+      </c>
+      <c r="F14" s="27" t="s">
+        <v>515</v>
+      </c>
+      <c r="G14" s="28">
+        <v>10</v>
+      </c>
+      <c r="H14" s="28">
+        <v>0</v>
+      </c>
+      <c r="I14" s="27">
+        <v>2.722</v>
+      </c>
+      <c r="J14" s="29">
+        <v>27.22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" s="2" customFormat="1">
+      <c r="A15" s="28">
+        <v>14</v>
+      </c>
+      <c r="B15" s="28">
+        <v>5</v>
+      </c>
+      <c r="C15" s="27" t="s">
+        <v>563</v>
+      </c>
+      <c r="D15" s="27" t="s">
+        <v>562</v>
+      </c>
+      <c r="E15" s="27" t="s">
+        <v>565</v>
+      </c>
+      <c r="F15" s="27" t="s">
+        <v>243</v>
+      </c>
+      <c r="G15" s="28">
+        <v>5</v>
+      </c>
+      <c r="H15" s="28">
+        <v>0</v>
+      </c>
+      <c r="I15" s="27">
+        <v>0.32400000000000001</v>
+      </c>
+      <c r="J15" s="29">
+        <v>1.62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" s="2" customFormat="1">
+      <c r="A16" s="28">
+        <v>15</v>
+      </c>
+      <c r="B16" s="28">
+        <v>10</v>
+      </c>
+      <c r="C16" s="27" t="s">
+        <v>317</v>
+      </c>
+      <c r="D16" s="27" t="s">
+        <v>313</v>
+      </c>
+      <c r="E16" s="27" t="s">
+        <v>316</v>
+      </c>
+      <c r="F16" s="27" t="s">
+        <v>315</v>
+      </c>
+      <c r="G16" s="28">
+        <v>10</v>
+      </c>
+      <c r="H16" s="28">
+        <v>0</v>
+      </c>
+      <c r="I16" s="27">
+        <v>0.753</v>
+      </c>
+      <c r="J16" s="29">
+        <v>7.53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" s="2" customFormat="1">
+      <c r="A17" s="28">
+        <v>16</v>
+      </c>
+      <c r="B17" s="28">
+        <v>10</v>
+      </c>
+      <c r="C17" s="27" t="s">
+        <v>311</v>
+      </c>
+      <c r="D17" s="27" t="s">
+        <v>306</v>
+      </c>
+      <c r="E17" s="27" t="s">
+        <v>310</v>
+      </c>
+      <c r="F17" s="27" t="s">
+        <v>309</v>
+      </c>
+      <c r="G17" s="28">
+        <v>10</v>
+      </c>
+      <c r="H17" s="28">
+        <v>0</v>
+      </c>
+      <c r="I17" s="27">
+        <v>0.59899999999999998</v>
+      </c>
+      <c r="J17" s="29">
+        <v>5.99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" s="2" customFormat="1">
+      <c r="A18" s="28">
+        <v>17</v>
+      </c>
+      <c r="B18" s="28">
+        <v>10</v>
+      </c>
+      <c r="C18" s="27" t="s">
+        <v>530</v>
+      </c>
+      <c r="D18" s="27" t="s">
+        <v>525</v>
+      </c>
+      <c r="E18" s="27" t="s">
+        <v>529</v>
+      </c>
+      <c r="F18" s="27" t="s">
+        <v>528</v>
+      </c>
+      <c r="G18" s="28">
+        <v>10</v>
+      </c>
+      <c r="H18" s="28">
+        <v>0</v>
+      </c>
+      <c r="I18" s="27">
+        <v>0.41099999999999998</v>
+      </c>
+      <c r="J18" s="29">
+        <v>4.1100000000000003</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" s="2" customFormat="1">
+      <c r="A19" s="28">
+        <v>18</v>
+      </c>
+      <c r="B19" s="28">
+        <v>200</v>
+      </c>
+      <c r="C19" s="27" t="s">
+        <v>207</v>
+      </c>
+      <c r="D19" s="27" t="s">
+        <v>208</v>
+      </c>
+      <c r="E19" s="27" t="s">
+        <v>570</v>
+      </c>
+      <c r="F19" s="27" t="s">
+        <v>205</v>
+      </c>
+      <c r="G19" s="28">
+        <v>200</v>
+      </c>
+      <c r="H19" s="28">
+        <v>0</v>
+      </c>
+      <c r="I19" s="27">
+        <v>2.4299999999999999E-2</v>
+      </c>
+      <c r="J19" s="29">
+        <v>4.8600000000000003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" s="2" customFormat="1">
+      <c r="A20" s="28">
+        <v>19</v>
+      </c>
+      <c r="B20" s="28">
+        <v>10</v>
+      </c>
+      <c r="C20" s="27" t="s">
+        <v>158</v>
+      </c>
+      <c r="D20" s="27" t="s">
+        <v>159</v>
+      </c>
+      <c r="E20" s="27" t="s">
+        <v>157</v>
+      </c>
+      <c r="F20" s="27" t="s">
+        <v>156</v>
+      </c>
+      <c r="G20" s="28">
+        <v>10</v>
+      </c>
+      <c r="H20" s="28">
+        <v>0</v>
+      </c>
+      <c r="I20" s="27">
+        <v>0.88100000000000001</v>
+      </c>
+      <c r="J20" s="29">
+        <v>8.81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" s="2" customFormat="1">
+      <c r="A21" s="28">
+        <v>20</v>
+      </c>
+      <c r="B21" s="28">
+        <v>20</v>
+      </c>
+      <c r="C21" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" s="27" t="s">
+        <v>201</v>
+      </c>
+      <c r="G21" s="28">
+        <v>20</v>
+      </c>
+      <c r="H21" s="28">
+        <v>0</v>
+      </c>
+      <c r="I21" s="27">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="J21" s="29">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" s="2" customFormat="1">
+      <c r="A22" s="28">
+        <v>21</v>
+      </c>
+      <c r="B22" s="28">
+        <v>100</v>
+      </c>
+      <c r="C22" s="27" t="s">
+        <v>330</v>
+      </c>
+      <c r="D22" s="27" t="s">
+        <v>331</v>
+      </c>
+      <c r="E22" s="27" t="s">
+        <v>329</v>
+      </c>
+      <c r="F22" s="27" t="s">
+        <v>328</v>
+      </c>
+      <c r="G22" s="28">
+        <v>100</v>
+      </c>
+      <c r="H22" s="28">
+        <v>0</v>
+      </c>
+      <c r="I22" s="27">
+        <v>0.25679999999999997</v>
+      </c>
+      <c r="J22" s="29">
+        <v>25.68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" s="2" customFormat="1">
+      <c r="A23" s="28">
+        <v>22</v>
+      </c>
+      <c r="B23" s="28">
+        <v>3</v>
+      </c>
+      <c r="C23" s="27" t="s">
+        <v>537</v>
+      </c>
+      <c r="D23" s="27" t="s">
+        <v>538</v>
+      </c>
+      <c r="E23" s="27" t="s">
+        <v>536</v>
+      </c>
+      <c r="F23" s="27" t="s">
+        <v>535</v>
+      </c>
+      <c r="G23" s="28">
+        <v>3</v>
+      </c>
+      <c r="H23" s="28">
+        <v>0</v>
+      </c>
+      <c r="I23" s="27">
+        <v>1.23</v>
+      </c>
+      <c r="J23" s="29">
+        <v>3.69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" s="2" customFormat="1">
+      <c r="A24" s="28">
+        <v>23</v>
+      </c>
+      <c r="B24" s="28">
+        <v>10</v>
+      </c>
+      <c r="C24" s="27" t="s">
+        <v>284</v>
+      </c>
+      <c r="D24" s="27" t="s">
+        <v>285</v>
+      </c>
+      <c r="E24" s="27" t="s">
+        <v>283</v>
+      </c>
+      <c r="F24" s="27" t="s">
+        <v>282</v>
+      </c>
+      <c r="G24" s="28">
+        <v>10</v>
+      </c>
+      <c r="H24" s="28">
+        <v>0</v>
+      </c>
+      <c r="I24" s="27">
+        <v>0.39200000000000002</v>
+      </c>
+      <c r="J24" s="29">
+        <v>3.92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" s="2" customFormat="1">
+      <c r="A25" s="28">
+        <v>24</v>
+      </c>
+      <c r="B25" s="28">
+        <v>4</v>
+      </c>
+      <c r="C25" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="D25" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="E25" s="27" t="s">
+        <v>117</v>
+      </c>
+      <c r="F25" s="27" t="s">
+        <v>446</v>
+      </c>
+      <c r="G25" s="28">
+        <v>4</v>
+      </c>
+      <c r="H25" s="28">
+        <v>0</v>
+      </c>
+      <c r="I25" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="J25" s="29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" s="2" customFormat="1">
+      <c r="A26" s="28">
+        <v>25</v>
+      </c>
+      <c r="B26" s="28">
+        <v>4</v>
+      </c>
+      <c r="C26" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="E26" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="F26" s="27" t="s">
+        <v>290</v>
+      </c>
+      <c r="G26" s="28">
+        <v>4</v>
+      </c>
+      <c r="H26" s="28">
+        <v>0</v>
+      </c>
+      <c r="I26" s="27">
+        <v>2.5299999999999998</v>
+      </c>
+      <c r="J26" s="29">
+        <v>10.119999999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" s="2" customFormat="1">
+      <c r="A27" s="28">
+        <v>26</v>
+      </c>
+      <c r="B27" s="28">
+        <v>15</v>
+      </c>
+      <c r="C27" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="D27" s="27" t="s">
+        <v>167</v>
+      </c>
+      <c r="E27" s="27" t="s">
+        <v>579</v>
+      </c>
+      <c r="F27" s="27" t="s">
+        <v>164</v>
+      </c>
+      <c r="G27" s="28">
+        <v>15</v>
+      </c>
+      <c r="H27" s="28">
+        <v>0</v>
+      </c>
+      <c r="I27" s="27">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="J27" s="29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" s="2" customFormat="1">
+      <c r="A28" s="28">
+        <v>27</v>
+      </c>
+      <c r="B28" s="28">
+        <v>10</v>
+      </c>
+      <c r="C28" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D28" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="E28" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="F28" s="27" t="s">
+        <v>505</v>
+      </c>
+      <c r="G28" s="28">
+        <v>10</v>
+      </c>
+      <c r="H28" s="28">
+        <v>0</v>
+      </c>
+      <c r="I28" s="27">
+        <v>1.5449999999999999</v>
+      </c>
+      <c r="J28" s="29">
+        <v>15.45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" s="2" customFormat="1">
+      <c r="A29" s="28">
+        <v>28</v>
+      </c>
+      <c r="B29" s="28">
+        <v>10</v>
+      </c>
+      <c r="C29" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="D29" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="F29" s="27" t="s">
+        <v>460</v>
+      </c>
+      <c r="G29" s="28">
+        <v>10</v>
+      </c>
+      <c r="H29" s="28">
+        <v>0</v>
+      </c>
+      <c r="I29" s="27">
+        <v>2.9039999999999999</v>
+      </c>
+      <c r="J29" s="29">
+        <v>29.04</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" s="2" customFormat="1">
+      <c r="A30" s="28">
+        <v>29</v>
+      </c>
+      <c r="B30" s="28">
+        <v>20</v>
+      </c>
+      <c r="C30" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="D30" s="28">
+        <v>824500500</v>
+      </c>
+      <c r="E30" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="F30" s="27" t="s">
+        <v>232</v>
+      </c>
+      <c r="G30" s="28">
+        <v>20</v>
+      </c>
+      <c r="H30" s="28">
+        <v>0</v>
+      </c>
+      <c r="I30" s="27">
+        <v>0.252</v>
+      </c>
+      <c r="J30" s="29">
+        <v>5.04</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" s="2" customFormat="1">
+      <c r="A31" s="28">
+        <v>30</v>
+      </c>
+      <c r="B31" s="28">
+        <v>10</v>
+      </c>
+      <c r="C31" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="D31" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="E31" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="F31" s="27" t="s">
+        <v>236</v>
+      </c>
+      <c r="G31" s="28">
+        <v>10</v>
+      </c>
+      <c r="H31" s="28">
+        <v>0</v>
+      </c>
+      <c r="I31" s="27">
+        <v>0.27400000000000002</v>
+      </c>
+      <c r="J31" s="29">
+        <v>2.74</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" s="2" customFormat="1">
+      <c r="A32" s="28">
+        <v>31</v>
+      </c>
+      <c r="B32" s="28">
+        <v>10</v>
+      </c>
+      <c r="C32" s="27" t="s">
+        <v>492</v>
+      </c>
+      <c r="D32" s="27" t="s">
+        <v>493</v>
+      </c>
+      <c r="E32" s="27" t="s">
+        <v>491</v>
+      </c>
+      <c r="F32" s="27" t="s">
+        <v>490</v>
+      </c>
+      <c r="G32" s="28">
+        <v>10</v>
+      </c>
+      <c r="H32" s="28">
+        <v>0</v>
+      </c>
+      <c r="I32" s="27">
+        <v>7.343</v>
+      </c>
+      <c r="J32" s="29">
+        <v>73.430000000000007</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" s="2" customFormat="1">
+      <c r="A33" s="28">
+        <v>32</v>
+      </c>
+      <c r="B33" s="28">
+        <v>100</v>
+      </c>
+      <c r="C33" s="27" t="s">
+        <v>226</v>
+      </c>
+      <c r="D33" s="27" t="s">
+        <v>227</v>
+      </c>
+      <c r="E33" s="27" t="s">
+        <v>225</v>
+      </c>
+      <c r="F33" s="27" t="s">
+        <v>224</v>
+      </c>
+      <c r="G33" s="28">
+        <v>81</v>
+      </c>
+      <c r="H33" s="28">
+        <v>19</v>
+      </c>
+      <c r="I33" s="27">
+        <v>7.8700000000000006E-2</v>
+      </c>
+      <c r="J33" s="29">
+        <v>7.87</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" s="2" customFormat="1">
+      <c r="A34" s="28">
+        <v>33</v>
+      </c>
+      <c r="B34" s="28">
+        <v>10</v>
+      </c>
+      <c r="C34" s="27" t="s">
+        <v>174</v>
+      </c>
+      <c r="D34" s="27" t="s">
+        <v>175</v>
+      </c>
+      <c r="E34" s="27" t="s">
+        <v>587</v>
+      </c>
+      <c r="F34" s="27" t="s">
+        <v>172</v>
+      </c>
+      <c r="G34" s="28">
+        <v>10</v>
+      </c>
+      <c r="H34" s="28">
+        <v>0</v>
+      </c>
+      <c r="I34" s="27">
+        <v>0.27700000000000002</v>
+      </c>
+      <c r="J34" s="29">
+        <v>2.77</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" s="2" customFormat="1">
+      <c r="A35" s="28">
+        <v>34</v>
+      </c>
+      <c r="B35" s="28">
+        <v>20</v>
+      </c>
+      <c r="C35" s="27" t="s">
+        <v>589</v>
+      </c>
+      <c r="D35" s="27" t="s">
+        <v>588</v>
+      </c>
+      <c r="E35" s="27" t="s">
+        <v>591</v>
+      </c>
+      <c r="F35" s="27" t="s">
+        <v>147</v>
+      </c>
+      <c r="G35" s="28">
+        <v>20</v>
+      </c>
+      <c r="H35" s="28">
+        <v>0</v>
+      </c>
+      <c r="I35" s="27">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="J35" s="29">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" s="2" customFormat="1">
+      <c r="A36" s="28">
+        <v>35</v>
+      </c>
+      <c r="B36" s="28">
+        <v>20</v>
+      </c>
+      <c r="C36" s="27" t="s">
+        <v>323</v>
+      </c>
+      <c r="D36" s="27" t="s">
+        <v>324</v>
+      </c>
+      <c r="E36" s="27" t="s">
+        <v>593</v>
+      </c>
+      <c r="F36" s="27" t="s">
+        <v>321</v>
+      </c>
+      <c r="G36" s="28">
+        <v>20</v>
+      </c>
+      <c r="H36" s="28">
+        <v>0</v>
+      </c>
+      <c r="I36" s="27">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="J36" s="29">
+        <v>1.84</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" s="2" customFormat="1">
+      <c r="A37" s="28">
+        <v>36</v>
+      </c>
+      <c r="B37" s="28">
+        <v>10</v>
+      </c>
+      <c r="C37" s="27" t="s">
+        <v>336</v>
+      </c>
+      <c r="D37" s="27" t="s">
+        <v>337</v>
+      </c>
+      <c r="E37" s="27" t="s">
+        <v>595</v>
+      </c>
+      <c r="F37" s="27" t="s">
+        <v>334</v>
+      </c>
+      <c r="G37" s="28">
+        <v>10</v>
+      </c>
+      <c r="H37" s="28">
+        <v>0</v>
+      </c>
+      <c r="I37" s="27">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="J37" s="29">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" s="2" customFormat="1">
+      <c r="A38" s="28">
+        <v>37</v>
+      </c>
+      <c r="B38" s="28">
+        <v>20</v>
+      </c>
+      <c r="C38" s="27" t="s">
+        <v>400</v>
+      </c>
+      <c r="D38" s="27" t="s">
+        <v>401</v>
+      </c>
+      <c r="E38" s="27" t="s">
+        <v>596</v>
+      </c>
+      <c r="F38" s="27" t="s">
+        <v>398</v>
+      </c>
+      <c r="G38" s="28">
+        <v>20</v>
+      </c>
+      <c r="H38" s="28">
+        <v>0</v>
+      </c>
+      <c r="I38" s="27">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="J38" s="29">
+        <v>1.1599999999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" s="2" customFormat="1">
+      <c r="A39" s="28">
+        <v>38</v>
+      </c>
+      <c r="B39" s="28">
+        <v>20</v>
+      </c>
+      <c r="C39" s="27" t="s">
+        <v>374</v>
+      </c>
+      <c r="D39" s="27" t="s">
+        <v>375</v>
+      </c>
+      <c r="E39" s="27" t="s">
+        <v>598</v>
+      </c>
+      <c r="F39" s="27" t="s">
+        <v>372</v>
+      </c>
+      <c r="G39" s="28">
+        <v>20</v>
+      </c>
+      <c r="H39" s="28">
+        <v>0</v>
+      </c>
+      <c r="I39" s="27">
+        <v>0.26</v>
+      </c>
+      <c r="J39" s="29">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" s="2" customFormat="1">
+      <c r="A40" s="28">
+        <v>39</v>
+      </c>
+      <c r="B40" s="28">
+        <v>100</v>
+      </c>
+      <c r="C40" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="D40" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="E40" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="F40" s="27" t="s">
+        <v>359</v>
+      </c>
+      <c r="G40" s="28">
+        <v>100</v>
+      </c>
+      <c r="H40" s="28">
+        <v>0</v>
+      </c>
+      <c r="I40" s="27">
+        <v>6.4999999999999997E-3</v>
+      </c>
+      <c r="J40" s="29">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" s="2" customFormat="1">
+      <c r="A41" s="28">
+        <v>40</v>
+      </c>
+      <c r="B41" s="28">
+        <v>100</v>
+      </c>
+      <c r="C41" s="27" t="s">
+        <v>369</v>
+      </c>
+      <c r="D41" s="27" t="s">
+        <v>370</v>
+      </c>
+      <c r="E41" s="27" t="s">
+        <v>601</v>
+      </c>
+      <c r="F41" s="27" t="s">
+        <v>367</v>
+      </c>
+      <c r="G41" s="28">
+        <v>100</v>
+      </c>
+      <c r="H41" s="28">
+        <v>0</v>
+      </c>
+      <c r="I41" s="27">
+        <v>2.2700000000000001E-2</v>
+      </c>
+      <c r="J41" s="29">
+        <v>2.27</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" s="2" customFormat="1">
+      <c r="A42" s="28">
+        <v>41</v>
+      </c>
+      <c r="B42" s="28">
+        <v>100</v>
+      </c>
+      <c r="C42" s="27" t="s">
+        <v>389</v>
+      </c>
+      <c r="D42" s="27" t="s">
+        <v>390</v>
+      </c>
+      <c r="E42" s="27" t="s">
+        <v>603</v>
+      </c>
+      <c r="F42" s="27" t="s">
+        <v>387</v>
+      </c>
+      <c r="G42" s="28">
+        <v>100</v>
+      </c>
+      <c r="H42" s="28">
+        <v>0</v>
+      </c>
+      <c r="I42" s="27">
+        <v>2.2700000000000001E-2</v>
+      </c>
+      <c r="J42" s="29">
+        <v>2.27</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" s="2" customFormat="1">
+      <c r="A43" s="28">
+        <v>42</v>
+      </c>
+      <c r="B43" s="28">
+        <v>100</v>
+      </c>
+      <c r="C43" s="27" t="s">
+        <v>363</v>
+      </c>
+      <c r="D43" s="27" t="s">
+        <v>364</v>
+      </c>
+      <c r="E43" s="27" t="s">
+        <v>605</v>
+      </c>
+      <c r="F43" s="27" t="s">
+        <v>361</v>
+      </c>
+      <c r="G43" s="28">
+        <v>100</v>
+      </c>
+      <c r="H43" s="28">
+        <v>0</v>
+      </c>
+      <c r="I43" s="27">
+        <v>2.3599999999999999E-2</v>
+      </c>
+      <c r="J43" s="29">
+        <v>2.36</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" s="2" customFormat="1">
+      <c r="A44" s="28">
+        <v>43</v>
+      </c>
+      <c r="B44" s="28">
+        <v>100</v>
+      </c>
+      <c r="C44" s="27" t="s">
+        <v>342</v>
+      </c>
+      <c r="D44" s="27" t="s">
+        <v>343</v>
+      </c>
+      <c r="E44" s="27" t="s">
+        <v>341</v>
+      </c>
+      <c r="F44" s="27" t="s">
+        <v>340</v>
+      </c>
+      <c r="G44" s="28">
+        <v>100</v>
+      </c>
+      <c r="H44" s="28">
+        <v>0</v>
+      </c>
+      <c r="I44" s="27">
+        <v>0.10150000000000001</v>
+      </c>
+      <c r="J44" s="29">
+        <v>10.15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" s="2" customFormat="1">
+      <c r="A45" s="28">
+        <v>44</v>
+      </c>
+      <c r="B45" s="28">
+        <v>10</v>
+      </c>
+      <c r="C45" s="27" t="s">
+        <v>348</v>
+      </c>
+      <c r="D45" s="27" t="s">
+        <v>349</v>
+      </c>
+      <c r="E45" s="27" t="s">
+        <v>608</v>
+      </c>
+      <c r="F45" s="27" t="s">
+        <v>346</v>
+      </c>
+      <c r="G45" s="28">
+        <v>10</v>
+      </c>
+      <c r="H45" s="28">
+        <v>0</v>
+      </c>
+      <c r="I45" s="27">
+        <v>0.26</v>
+      </c>
+      <c r="J45" s="29">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" s="2" customFormat="1">
+      <c r="A46" s="28">
+        <v>45</v>
+      </c>
+      <c r="B46" s="28">
+        <v>3</v>
+      </c>
+      <c r="C46" s="27" t="s">
+        <v>468</v>
+      </c>
+      <c r="D46" s="27" t="s">
+        <v>469</v>
+      </c>
+      <c r="E46" s="27" t="s">
+        <v>467</v>
+      </c>
+      <c r="F46" s="27" t="s">
+        <v>466</v>
+      </c>
+      <c r="G46" s="28">
+        <v>3</v>
+      </c>
+      <c r="H46" s="28">
+        <v>0</v>
+      </c>
+      <c r="I46" s="27">
+        <v>0.84</v>
+      </c>
+      <c r="J46" s="29">
+        <v>2.52</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" s="2" customFormat="1">
+      <c r="A47" s="28">
+        <v>46</v>
+      </c>
+      <c r="B47" s="28">
+        <v>3</v>
+      </c>
+      <c r="C47" s="27" t="s">
+        <v>500</v>
+      </c>
+      <c r="D47" s="27" t="s">
+        <v>501</v>
+      </c>
+      <c r="E47" s="27" t="s">
+        <v>499</v>
+      </c>
+      <c r="F47" s="27" t="s">
+        <v>498</v>
+      </c>
+      <c r="G47" s="28">
+        <v>3</v>
+      </c>
+      <c r="H47" s="28">
+        <v>0</v>
+      </c>
+      <c r="I47" s="27">
+        <v>0.41</v>
+      </c>
+      <c r="J47" s="29">
+        <v>1.23</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" s="2" customFormat="1">
+      <c r="A48" s="28">
+        <v>47</v>
+      </c>
+      <c r="B48" s="28">
+        <v>10</v>
+      </c>
+      <c r="C48" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="D48" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="E48" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="F48" s="27" t="s">
+        <v>213</v>
+      </c>
+      <c r="G48" s="28">
+        <v>10</v>
+      </c>
+      <c r="H48" s="28">
+        <v>0</v>
+      </c>
+      <c r="I48" s="27">
+        <v>0.72199999999999998</v>
+      </c>
+      <c r="J48" s="29">
+        <v>7.22</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" s="2" customFormat="1">
+      <c r="A49" s="28">
+        <v>48</v>
+      </c>
+      <c r="B49" s="28">
+        <v>20</v>
+      </c>
+      <c r="C49" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="D49" s="28">
+        <v>74279220181</v>
+      </c>
+      <c r="E49" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="F49" s="27" t="s">
+        <v>261</v>
+      </c>
+      <c r="G49" s="28">
+        <v>20</v>
+      </c>
+      <c r="H49" s="28">
+        <v>0</v>
+      </c>
+      <c r="I49" s="27">
+        <v>0.32</v>
+      </c>
+      <c r="J49" s="29">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" s="2" customFormat="1">
+      <c r="A50" s="28">
+        <v>49</v>
+      </c>
+      <c r="B50" s="28">
+        <v>3</v>
+      </c>
+      <c r="C50" s="27" t="s">
+        <v>510</v>
+      </c>
+      <c r="D50" s="27" t="s">
+        <v>511</v>
+      </c>
+      <c r="E50" s="27" t="s">
+        <v>475</v>
+      </c>
+      <c r="F50" s="27" t="s">
+        <v>508</v>
+      </c>
+      <c r="G50" s="28">
+        <v>3</v>
+      </c>
+      <c r="H50" s="28">
+        <v>0</v>
+      </c>
+      <c r="I50" s="27">
+        <v>4.57</v>
+      </c>
+      <c r="J50" s="29">
+        <v>13.71</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" s="2" customFormat="1">
+      <c r="A51" s="28">
+        <v>50</v>
+      </c>
+      <c r="B51" s="28">
+        <v>50</v>
+      </c>
+      <c r="C51" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="D51" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="E51" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="F51" s="27" t="s">
+        <v>191</v>
+      </c>
+      <c r="G51" s="28">
+        <v>50</v>
+      </c>
+      <c r="H51" s="28">
+        <v>0</v>
+      </c>
+      <c r="I51" s="27">
+        <v>2.4799999999999999E-2</v>
+      </c>
+      <c r="J51" s="29">
+        <v>1.24</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" s="2" customFormat="1">
+      <c r="A52" s="28">
+        <v>51</v>
+      </c>
+      <c r="B52" s="28">
+        <v>100</v>
+      </c>
+      <c r="C52" s="27" t="s">
+        <v>354</v>
+      </c>
+      <c r="D52" s="27" t="s">
+        <v>355</v>
+      </c>
+      <c r="E52" s="27" t="s">
+        <v>353</v>
+      </c>
+      <c r="F52" s="27" t="s">
+        <v>352</v>
+      </c>
+      <c r="G52" s="28">
+        <v>100</v>
+      </c>
+      <c r="H52" s="28">
+        <v>0</v>
+      </c>
+      <c r="I52" s="27">
+        <v>7.5700000000000003E-2</v>
+      </c>
+      <c r="J52" s="29">
+        <v>7.57</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" s="2" customFormat="1">
+      <c r="A53" s="28">
+        <v>52</v>
+      </c>
+      <c r="B53" s="28">
+        <v>25</v>
+      </c>
+      <c r="C53" s="27" t="s">
+        <v>254</v>
+      </c>
+      <c r="D53" s="27" t="s">
+        <v>255</v>
+      </c>
+      <c r="E53" s="27" t="s">
+        <v>568</v>
+      </c>
+      <c r="F53" s="27" t="s">
+        <v>252</v>
+      </c>
+      <c r="G53" s="28">
+        <v>25</v>
+      </c>
+      <c r="H53" s="28">
+        <v>0</v>
+      </c>
+      <c r="I53" s="27">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="J53" s="29">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" s="2" customFormat="1">
+      <c r="A54" s="28">
+        <v>53</v>
+      </c>
+      <c r="B54" s="28">
+        <v>10</v>
+      </c>
+      <c r="C54" s="27" t="s">
+        <v>187</v>
+      </c>
+      <c r="D54" s="27" t="s">
+        <v>188</v>
+      </c>
+      <c r="E54" s="27" t="s">
+        <v>585</v>
+      </c>
+      <c r="F54" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="G54" s="28">
+        <v>10</v>
+      </c>
+      <c r="H54" s="28">
+        <v>0</v>
+      </c>
+      <c r="I54" s="27">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="J54" s="29">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" s="2" customFormat="1">
+      <c r="A55" s="28">
+        <v>54</v>
+      </c>
+      <c r="B55" s="28">
+        <v>100</v>
+      </c>
+      <c r="C55" s="27" t="s">
+        <v>618</v>
+      </c>
+      <c r="D55" s="27" t="s">
+        <v>617</v>
+      </c>
+      <c r="E55" s="27" t="s">
+        <v>379</v>
+      </c>
+      <c r="F55" s="27" t="s">
+        <v>378</v>
+      </c>
+      <c r="G55" s="28">
+        <v>100</v>
+      </c>
+      <c r="H55" s="28">
+        <v>0</v>
+      </c>
+      <c r="I55" s="27">
+        <v>0.10730000000000001</v>
+      </c>
+      <c r="J55" s="29">
+        <v>10.73</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" s="2" customFormat="1">
+      <c r="A56" s="28">
+        <v>55</v>
+      </c>
+      <c r="B56" s="28">
+        <v>10</v>
+      </c>
+      <c r="C56" s="27" t="s">
+        <v>621</v>
+      </c>
+      <c r="D56" s="27" t="s">
+        <v>620</v>
+      </c>
+      <c r="E56" s="27" t="s">
+        <v>623</v>
+      </c>
+      <c r="F56" s="27" t="s">
+        <v>384</v>
+      </c>
+      <c r="G56" s="28">
+        <v>10</v>
+      </c>
+      <c r="H56" s="28">
+        <v>0</v>
+      </c>
+      <c r="I56" s="27">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="J56" s="29">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" s="2" customFormat="1">
+      <c r="A57" s="28">
+        <v>56</v>
+      </c>
+      <c r="B57" s="28">
+        <v>100</v>
+      </c>
+      <c r="C57" s="27" t="s">
+        <v>639</v>
+      </c>
+      <c r="D57" s="27" t="s">
+        <v>640</v>
+      </c>
+      <c r="E57" s="27" t="s">
+        <v>641</v>
+      </c>
+      <c r="F57" s="27"/>
+      <c r="G57" s="28">
+        <v>100</v>
+      </c>
+      <c r="H57" s="28">
+        <v>0</v>
+      </c>
+      <c r="I57" s="27">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="J57" s="29">
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" s="2" customFormat="1">
+      <c r="A58" s="28">
+        <v>57</v>
+      </c>
+      <c r="B58" s="28">
+        <v>20</v>
+      </c>
+      <c r="C58" s="27" t="s">
+        <v>642</v>
+      </c>
+      <c r="D58" s="27" t="s">
+        <v>643</v>
+      </c>
+      <c r="E58" s="27" t="s">
+        <v>644</v>
+      </c>
+      <c r="F58" s="27"/>
+      <c r="G58" s="28">
+        <v>20</v>
+      </c>
+      <c r="H58" s="28">
+        <v>0</v>
+      </c>
+      <c r="I58" s="27">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="J58" s="29">
+        <v>3.88</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" s="2" customFormat="1">
+      <c r="A59" s="28">
+        <v>58</v>
+      </c>
+      <c r="B59" s="28">
+        <v>10</v>
+      </c>
+      <c r="C59" s="27" t="s">
+        <v>645</v>
+      </c>
+      <c r="D59" s="27" t="s">
+        <v>646</v>
+      </c>
+      <c r="E59" s="27" t="s">
+        <v>647</v>
+      </c>
+      <c r="F59" s="27" t="s">
+        <v>648</v>
+      </c>
+      <c r="G59" s="28">
+        <v>10</v>
+      </c>
+      <c r="H59" s="28">
+        <v>0</v>
+      </c>
+      <c r="I59" s="27">
+        <v>0.221</v>
+      </c>
+      <c r="J59" s="29">
+        <v>2.21</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" s="2" customFormat="1">
+      <c r="A60" s="28">
+        <v>59</v>
+      </c>
+      <c r="B60" s="28">
+        <v>1</v>
+      </c>
+      <c r="C60" s="27" t="s">
+        <v>649</v>
+      </c>
+      <c r="D60" s="27" t="s">
+        <v>650</v>
+      </c>
+      <c r="E60" s="27" t="s">
+        <v>651</v>
+      </c>
+      <c r="F60" s="27"/>
+      <c r="G60" s="28">
+        <v>1</v>
+      </c>
+      <c r="H60" s="28">
+        <v>0</v>
+      </c>
+      <c r="I60" s="27">
+        <v>16.989999999999998</v>
+      </c>
+      <c r="J60" s="29">
+        <v>16.989999999999998</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" s="2" customFormat="1">
+      <c r="A61" s="28">
+        <v>60</v>
+      </c>
+      <c r="B61" s="28">
+        <v>1</v>
+      </c>
+      <c r="C61" s="27" t="s">
+        <v>652</v>
+      </c>
+      <c r="D61" s="27" t="s">
+        <v>653</v>
+      </c>
+      <c r="E61" s="27" t="s">
+        <v>654</v>
+      </c>
+      <c r="F61" s="27"/>
+      <c r="G61" s="28">
+        <v>1</v>
+      </c>
+      <c r="H61" s="28">
+        <v>0</v>
+      </c>
+      <c r="I61" s="27">
+        <v>20.57</v>
+      </c>
+      <c r="J61" s="29">
+        <v>20.57</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" s="2" customFormat="1">
+      <c r="A62" s="28">
+        <v>61</v>
+      </c>
+      <c r="B62" s="28">
+        <v>1</v>
+      </c>
+      <c r="C62" s="27" t="s">
+        <v>655</v>
+      </c>
+      <c r="D62" s="27" t="s">
+        <v>656</v>
+      </c>
+      <c r="E62" s="27" t="s">
+        <v>657</v>
+      </c>
+      <c r="F62" s="27"/>
+      <c r="G62" s="28">
+        <v>1</v>
+      </c>
+      <c r="H62" s="28">
+        <v>0</v>
+      </c>
+      <c r="I62" s="27">
+        <v>20.57</v>
+      </c>
+      <c r="J62" s="29">
+        <v>20.57</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" s="2" customFormat="1">
+      <c r="A63" s="28">
+        <v>62</v>
+      </c>
+      <c r="B63" s="28">
+        <v>50</v>
+      </c>
+      <c r="C63" s="27" t="s">
+        <v>659</v>
+      </c>
+      <c r="D63" s="27" t="s">
+        <v>660</v>
+      </c>
+      <c r="E63" s="27" t="s">
+        <v>661</v>
+      </c>
+      <c r="F63" s="27" t="s">
+        <v>194</v>
+      </c>
+      <c r="G63" s="28">
+        <v>50</v>
+      </c>
+      <c r="H63" s="28">
+        <v>0</v>
+      </c>
+      <c r="I63" s="27">
+        <v>0.32100000000000001</v>
+      </c>
+      <c r="J63" s="29">
+        <v>16.05</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10">
+      <c r="A64" s="28">
+        <v>63</v>
+      </c>
+      <c r="B64" s="28">
+        <v>20</v>
+      </c>
+      <c r="C64" s="27" t="s">
+        <v>662</v>
+      </c>
+      <c r="D64" s="27" t="s">
+        <v>663</v>
+      </c>
+      <c r="E64" s="27" t="s">
+        <v>664</v>
+      </c>
+      <c r="F64" s="27" t="s">
         <v>394</v>
       </c>
-      <c r="G12" s="30">
-        <v>10</v>
-      </c>
-      <c r="H12" s="30">
-        <v>0</v>
-      </c>
-      <c r="I12" s="2">
-        <v>0.26200000000000001</v>
-      </c>
-      <c r="J12" s="31">
-        <v>2.62</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" s="2" customFormat="1">
-      <c r="A13" s="30">
-        <v>12</v>
-      </c>
-      <c r="B13" s="30">
-        <v>2</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="G13" s="30">
-        <v>2</v>
-      </c>
-      <c r="H13" s="30">
-        <v>0</v>
-      </c>
-      <c r="I13" s="2">
-        <v>1.66</v>
-      </c>
-      <c r="J13" s="31">
-        <v>3.32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" s="2" customFormat="1">
-      <c r="A14" s="30">
-        <v>13</v>
-      </c>
-      <c r="B14" s="30">
-        <v>50</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>559</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>558</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="G14" s="30">
-        <v>50</v>
-      </c>
-      <c r="H14" s="30">
-        <v>0</v>
-      </c>
-      <c r="I14" s="2">
-        <v>0.72460000000000002</v>
-      </c>
-      <c r="J14" s="31">
-        <v>36.229999999999997</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" s="2" customFormat="1">
-      <c r="A15" s="30">
-        <v>14</v>
-      </c>
-      <c r="B15" s="30">
-        <v>10</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>517</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>518</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>516</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>515</v>
-      </c>
-      <c r="G15" s="30">
-        <v>10</v>
-      </c>
-      <c r="H15" s="30">
-        <v>0</v>
-      </c>
-      <c r="I15" s="2">
-        <v>2.722</v>
-      </c>
-      <c r="J15" s="31">
-        <v>27.22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" s="2" customFormat="1">
-      <c r="A16" s="30">
-        <v>15</v>
-      </c>
-      <c r="B16" s="30">
-        <v>5</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>563</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>562</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>565</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="G16" s="30">
-        <v>5</v>
-      </c>
-      <c r="H16" s="30">
-        <v>0</v>
-      </c>
-      <c r="I16" s="2">
-        <v>0.32400000000000001</v>
-      </c>
-      <c r="J16" s="31">
-        <v>1.62</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" s="2" customFormat="1">
-      <c r="A17" s="30">
-        <v>16</v>
-      </c>
-      <c r="B17" s="30">
-        <v>10</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>317</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="G17" s="30">
-        <v>10</v>
-      </c>
-      <c r="H17" s="30">
-        <v>0</v>
-      </c>
-      <c r="I17" s="2">
-        <v>0.753</v>
-      </c>
-      <c r="J17" s="31">
-        <v>7.53</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" s="2" customFormat="1">
-      <c r="A18" s="30">
-        <v>17</v>
-      </c>
-      <c r="B18" s="30">
-        <v>10</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="G18" s="30">
-        <v>10</v>
-      </c>
-      <c r="H18" s="30">
-        <v>0</v>
-      </c>
-      <c r="I18" s="2">
-        <v>0.59899999999999998</v>
-      </c>
-      <c r="J18" s="31">
-        <v>5.99</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" s="2" customFormat="1">
-      <c r="A19" s="30">
-        <v>18</v>
-      </c>
-      <c r="B19" s="30">
-        <v>10</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>530</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>525</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>529</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>528</v>
-      </c>
-      <c r="G19" s="30">
-        <v>10</v>
-      </c>
-      <c r="H19" s="30">
-        <v>0</v>
-      </c>
-      <c r="I19" s="2">
-        <v>0.41099999999999998</v>
-      </c>
-      <c r="J19" s="31">
-        <v>4.1100000000000003</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" s="2" customFormat="1">
-      <c r="A20" s="30">
-        <v>19</v>
-      </c>
-      <c r="B20" s="30">
-        <v>100</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>570</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="G20" s="30">
-        <v>100</v>
-      </c>
-      <c r="H20" s="30">
-        <v>0</v>
-      </c>
-      <c r="I20" s="2">
-        <v>2.4299999999999999E-2</v>
-      </c>
-      <c r="J20" s="31">
-        <v>2.4300000000000002</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" s="2" customFormat="1">
-      <c r="A21" s="30">
+      <c r="G64" s="28">
         <v>20</v>
       </c>
-      <c r="B21" s="30">
-        <v>10</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="G21" s="30">
-        <v>10</v>
-      </c>
-      <c r="H21" s="30">
-        <v>0</v>
-      </c>
-      <c r="I21" s="2">
-        <v>0.88100000000000001</v>
-      </c>
-      <c r="J21" s="31">
-        <v>8.81</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" s="2" customFormat="1">
-      <c r="A22" s="30">
-        <v>21</v>
-      </c>
-      <c r="B22" s="30">
-        <v>20</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="G22" s="30">
-        <v>20</v>
-      </c>
-      <c r="H22" s="30">
-        <v>0</v>
-      </c>
-      <c r="I22" s="2">
-        <v>0.16500000000000001</v>
-      </c>
-      <c r="J22" s="31">
-        <v>3.3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" s="2" customFormat="1">
-      <c r="A23" s="30">
-        <v>22</v>
-      </c>
-      <c r="B23" s="30">
-        <v>20</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="G23" s="30">
-        <v>20</v>
-      </c>
-      <c r="H23" s="30">
-        <v>0</v>
-      </c>
-      <c r="I23" s="2">
-        <v>0.49399999999999999</v>
-      </c>
-      <c r="J23" s="31">
-        <v>9.8800000000000008</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" s="2" customFormat="1">
-      <c r="A24" s="30">
-        <v>23</v>
-      </c>
-      <c r="B24" s="30">
-        <v>2</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>537</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>538</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>536</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>535</v>
-      </c>
-      <c r="G24" s="30">
-        <v>2</v>
-      </c>
-      <c r="H24" s="30">
-        <v>0</v>
-      </c>
-      <c r="I24" s="2">
-        <v>1.23</v>
-      </c>
-      <c r="J24" s="31">
-        <v>2.46</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" s="2" customFormat="1">
-      <c r="A25" s="30">
-        <v>24</v>
-      </c>
-      <c r="B25" s="30">
-        <v>10</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="G25" s="30">
-        <v>10</v>
-      </c>
-      <c r="H25" s="30">
-        <v>0</v>
-      </c>
-      <c r="I25" s="2">
-        <v>0.39200000000000002</v>
-      </c>
-      <c r="J25" s="31">
-        <v>3.92</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" s="2" customFormat="1">
-      <c r="A26" s="30">
-        <v>25</v>
-      </c>
-      <c r="B26" s="30">
-        <v>4</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>446</v>
-      </c>
-      <c r="G26" s="30">
-        <v>4</v>
-      </c>
-      <c r="H26" s="30">
-        <v>0</v>
-      </c>
-      <c r="I26" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="J26" s="31">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" s="2" customFormat="1">
-      <c r="A27" s="30">
-        <v>26</v>
-      </c>
-      <c r="B27" s="30">
-        <v>4</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="G27" s="30">
-        <v>4</v>
-      </c>
-      <c r="H27" s="30">
-        <v>0</v>
-      </c>
-      <c r="I27" s="2">
-        <v>2.5299999999999998</v>
-      </c>
-      <c r="J27" s="31">
-        <v>10.119999999999999</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" s="2" customFormat="1">
-      <c r="A28" s="30">
-        <v>27</v>
-      </c>
-      <c r="B28" s="30">
-        <v>15</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>579</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="G28" s="30">
-        <v>15</v>
-      </c>
-      <c r="H28" s="30">
-        <v>0</v>
-      </c>
-      <c r="I28" s="2">
-        <v>0.13300000000000001</v>
-      </c>
-      <c r="J28" s="31">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" s="2" customFormat="1">
-      <c r="A29" s="30">
-        <v>28</v>
-      </c>
-      <c r="B29" s="30">
-        <v>10</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>505</v>
-      </c>
-      <c r="G29" s="30">
-        <v>10</v>
-      </c>
-      <c r="H29" s="30">
-        <v>0</v>
-      </c>
-      <c r="I29" s="2">
-        <v>1.5449999999999999</v>
-      </c>
-      <c r="J29" s="31">
-        <v>15.45</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" s="2" customFormat="1">
-      <c r="A30" s="30">
-        <v>29</v>
-      </c>
-      <c r="B30" s="30">
-        <v>10</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>460</v>
-      </c>
-      <c r="G30" s="30">
-        <v>10</v>
-      </c>
-      <c r="H30" s="30">
-        <v>0</v>
-      </c>
-      <c r="I30" s="2">
-        <v>2.9039999999999999</v>
-      </c>
-      <c r="J30" s="31">
-        <v>29.04</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" s="2" customFormat="1">
-      <c r="A31" s="30">
-        <v>30</v>
-      </c>
-      <c r="B31" s="30">
-        <v>20</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D31" s="30">
-        <v>824500500</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="G31" s="30">
-        <v>20</v>
-      </c>
-      <c r="H31" s="30">
-        <v>0</v>
-      </c>
-      <c r="I31" s="2">
-        <v>0.252</v>
-      </c>
-      <c r="J31" s="31">
-        <v>5.04</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" s="2" customFormat="1">
-      <c r="A32" s="30">
-        <v>31</v>
-      </c>
-      <c r="B32" s="30">
-        <v>10</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="G32" s="30">
-        <v>10</v>
-      </c>
-      <c r="H32" s="30">
-        <v>0</v>
-      </c>
-      <c r="I32" s="2">
-        <v>0.27400000000000002</v>
-      </c>
-      <c r="J32" s="31">
-        <v>2.74</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" s="2" customFormat="1">
-      <c r="A33" s="30">
-        <v>32</v>
-      </c>
-      <c r="B33" s="30">
-        <v>10</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>492</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>493</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>491</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>490</v>
-      </c>
-      <c r="G33" s="30">
-        <v>10</v>
-      </c>
-      <c r="H33" s="30">
-        <v>0</v>
-      </c>
-      <c r="I33" s="2">
-        <v>7.343</v>
-      </c>
-      <c r="J33" s="31">
-        <v>73.430000000000007</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" s="2" customFormat="1">
-      <c r="A34" s="30">
-        <v>33</v>
-      </c>
-      <c r="B34" s="30">
-        <v>100</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="G34" s="30">
-        <v>81</v>
-      </c>
-      <c r="H34" s="30">
-        <v>19</v>
-      </c>
-      <c r="I34" s="2">
-        <v>7.8700000000000006E-2</v>
-      </c>
-      <c r="J34" s="31">
-        <v>7.87</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" s="2" customFormat="1">
-      <c r="A35" s="30">
-        <v>34</v>
-      </c>
-      <c r="B35" s="30">
-        <v>10</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>587</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="G35" s="30">
-        <v>10</v>
-      </c>
-      <c r="H35" s="30">
-        <v>0</v>
-      </c>
-      <c r="I35" s="2">
-        <v>0.27700000000000002</v>
-      </c>
-      <c r="J35" s="31">
-        <v>2.77</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" s="2" customFormat="1">
-      <c r="A36" s="30">
-        <v>35</v>
-      </c>
-      <c r="B36" s="30">
-        <v>20</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>589</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>588</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>591</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="G36" s="30">
-        <v>20</v>
-      </c>
-      <c r="H36" s="30">
-        <v>0</v>
-      </c>
-      <c r="I36" s="2">
-        <v>0.16500000000000001</v>
-      </c>
-      <c r="J36" s="31">
-        <v>3.3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" s="2" customFormat="1">
-      <c r="A37" s="30">
-        <v>36</v>
-      </c>
-      <c r="B37" s="30">
-        <v>20</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>593</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="G37" s="30">
-        <v>20</v>
-      </c>
-      <c r="H37" s="30">
-        <v>0</v>
-      </c>
-      <c r="I37" s="2">
-        <v>9.1999999999999998E-2</v>
-      </c>
-      <c r="J37" s="31">
-        <v>1.84</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" s="2" customFormat="1">
-      <c r="A38" s="30">
-        <v>37</v>
-      </c>
-      <c r="B38" s="30">
-        <v>10</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>595</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="G38" s="30">
-        <v>10</v>
-      </c>
-      <c r="H38" s="30">
-        <v>0</v>
-      </c>
-      <c r="I38" s="2">
-        <v>5.8000000000000003E-2</v>
-      </c>
-      <c r="J38" s="31">
-        <v>0.57999999999999996</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" s="2" customFormat="1">
-      <c r="A39" s="30">
-        <v>38</v>
-      </c>
-      <c r="B39" s="30">
-        <v>10</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>401</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>596</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>398</v>
-      </c>
-      <c r="G39" s="30">
-        <v>10</v>
-      </c>
-      <c r="H39" s="30">
-        <v>0</v>
-      </c>
-      <c r="I39" s="2">
-        <v>5.8000000000000003E-2</v>
-      </c>
-      <c r="J39" s="31">
-        <v>0.57999999999999996</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" s="2" customFormat="1">
-      <c r="A40" s="30">
-        <v>39</v>
-      </c>
-      <c r="B40" s="30">
-        <v>20</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>375</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>598</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>372</v>
-      </c>
-      <c r="G40" s="30">
-        <v>20</v>
-      </c>
-      <c r="H40" s="30">
-        <v>0</v>
-      </c>
-      <c r="I40" s="2">
-        <v>0.26</v>
-      </c>
-      <c r="J40" s="31">
-        <v>5.2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" s="2" customFormat="1">
-      <c r="A41" s="30">
-        <v>40</v>
-      </c>
-      <c r="B41" s="30">
-        <v>100</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="G41" s="30">
-        <v>100</v>
-      </c>
-      <c r="H41" s="30">
-        <v>0</v>
-      </c>
-      <c r="I41" s="2">
-        <v>6.4999999999999997E-3</v>
-      </c>
-      <c r="J41" s="31">
-        <v>0.65</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" s="2" customFormat="1">
-      <c r="A42" s="30">
-        <v>41</v>
-      </c>
-      <c r="B42" s="30">
-        <v>100</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>370</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>601</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="G42" s="30">
-        <v>100</v>
-      </c>
-      <c r="H42" s="30">
-        <v>0</v>
-      </c>
-      <c r="I42" s="2">
-        <v>2.2700000000000001E-2</v>
-      </c>
-      <c r="J42" s="31">
-        <v>2.27</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" s="2" customFormat="1">
-      <c r="A43" s="30">
-        <v>42</v>
-      </c>
-      <c r="B43" s="30">
-        <v>100</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>390</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>603</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>387</v>
-      </c>
-      <c r="G43" s="30">
-        <v>100</v>
-      </c>
-      <c r="H43" s="30">
-        <v>0</v>
-      </c>
-      <c r="I43" s="2">
-        <v>2.2700000000000001E-2</v>
-      </c>
-      <c r="J43" s="31">
-        <v>2.27</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" s="2" customFormat="1">
-      <c r="A44" s="30">
-        <v>43</v>
-      </c>
-      <c r="B44" s="30">
-        <v>100</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>363</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>605</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>361</v>
-      </c>
-      <c r="G44" s="30">
-        <v>100</v>
-      </c>
-      <c r="H44" s="30">
-        <v>0</v>
-      </c>
-      <c r="I44" s="2">
-        <v>2.3599999999999999E-2</v>
-      </c>
-      <c r="J44" s="31">
-        <v>2.36</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" s="2" customFormat="1">
-      <c r="A45" s="30">
-        <v>44</v>
-      </c>
-      <c r="B45" s="30">
-        <v>100</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>343</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>340</v>
-      </c>
-      <c r="G45" s="30">
-        <v>100</v>
-      </c>
-      <c r="H45" s="30">
-        <v>0</v>
-      </c>
-      <c r="I45" s="2">
-        <v>0.10150000000000001</v>
-      </c>
-      <c r="J45" s="31">
-        <v>10.15</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" s="2" customFormat="1">
-      <c r="A46" s="30">
-        <v>45</v>
-      </c>
-      <c r="B46" s="30">
-        <v>10</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>348</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>349</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>608</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>346</v>
-      </c>
-      <c r="G46" s="30">
-        <v>10</v>
-      </c>
-      <c r="H46" s="30">
-        <v>0</v>
-      </c>
-      <c r="I46" s="2">
-        <v>0.26</v>
-      </c>
-      <c r="J46" s="31">
-        <v>2.6</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" s="2" customFormat="1">
-      <c r="A47" s="30">
-        <v>46</v>
-      </c>
-      <c r="B47" s="30">
-        <v>3</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>468</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>469</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>467</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>466</v>
-      </c>
-      <c r="G47" s="30">
-        <v>3</v>
-      </c>
-      <c r="H47" s="30">
-        <v>0</v>
-      </c>
-      <c r="I47" s="2">
-        <v>0.84</v>
-      </c>
-      <c r="J47" s="31">
-        <v>2.52</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" s="2" customFormat="1">
-      <c r="A48" s="30">
-        <v>47</v>
-      </c>
-      <c r="B48" s="30">
-        <v>3</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>500</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>501</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>499</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>498</v>
-      </c>
-      <c r="G48" s="30">
-        <v>3</v>
-      </c>
-      <c r="H48" s="30">
-        <v>0</v>
-      </c>
-      <c r="I48" s="2">
-        <v>0.41</v>
-      </c>
-      <c r="J48" s="31">
-        <v>1.23</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" s="2" customFormat="1">
-      <c r="A49" s="30">
-        <v>48</v>
-      </c>
-      <c r="B49" s="30">
-        <v>10</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="G49" s="30">
-        <v>10</v>
-      </c>
-      <c r="H49" s="30">
-        <v>0</v>
-      </c>
-      <c r="I49" s="2">
-        <v>0.72199999999999998</v>
-      </c>
-      <c r="J49" s="31">
-        <v>7.22</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" s="2" customFormat="1">
-      <c r="A50" s="30">
-        <v>49</v>
-      </c>
-      <c r="B50" s="30">
-        <v>20</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D50" s="30">
-        <v>74279220181</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="G50" s="30">
-        <v>20</v>
-      </c>
-      <c r="H50" s="30">
-        <v>0</v>
-      </c>
-      <c r="I50" s="2">
-        <v>0.32</v>
-      </c>
-      <c r="J50" s="31">
-        <v>6.4</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" s="2" customFormat="1">
-      <c r="A51" s="30">
-        <v>50</v>
-      </c>
-      <c r="B51" s="30">
-        <v>3</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>510</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>511</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>475</v>
-      </c>
-      <c r="F51" s="2" t="s">
-        <v>508</v>
-      </c>
-      <c r="G51" s="30">
-        <v>3</v>
-      </c>
-      <c r="H51" s="30">
-        <v>0</v>
-      </c>
-      <c r="I51" s="2">
-        <v>4.57</v>
-      </c>
-      <c r="J51" s="31">
-        <v>13.71</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" s="2" customFormat="1">
-      <c r="A52" s="30">
-        <v>51</v>
-      </c>
-      <c r="B52" s="30">
-        <v>50</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="F52" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="G52" s="30">
-        <v>50</v>
-      </c>
-      <c r="H52" s="30">
-        <v>0</v>
-      </c>
-      <c r="I52" s="2">
-        <v>2.4799999999999999E-2</v>
-      </c>
-      <c r="J52" s="31">
-        <v>1.24</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" s="2" customFormat="1">
-      <c r="A53" s="30">
-        <v>52</v>
-      </c>
-      <c r="B53" s="30">
-        <v>100</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>354</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>353</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>352</v>
-      </c>
-      <c r="G53" s="30">
-        <v>100</v>
-      </c>
-      <c r="H53" s="30">
-        <v>0</v>
-      </c>
-      <c r="I53" s="2">
-        <v>7.5700000000000003E-2</v>
-      </c>
-      <c r="J53" s="31">
-        <v>7.57</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" s="2" customFormat="1">
-      <c r="A54" s="30">
-        <v>53</v>
-      </c>
-      <c r="B54" s="30">
-        <v>25</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>568</v>
-      </c>
-      <c r="F54" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="G54" s="30">
-        <v>25</v>
-      </c>
-      <c r="H54" s="30">
-        <v>0</v>
-      </c>
-      <c r="I54" s="2">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="J54" s="31">
-        <v>1.75</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" s="2" customFormat="1">
-      <c r="A55" s="30">
-        <v>54</v>
-      </c>
-      <c r="B55" s="30">
-        <v>10</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>585</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="G55" s="30">
-        <v>10</v>
-      </c>
-      <c r="H55" s="30">
-        <v>0</v>
-      </c>
-      <c r="I55" s="2">
-        <v>3.7999999999999999E-2</v>
-      </c>
-      <c r="J55" s="31">
-        <v>0.38</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" s="2" customFormat="1">
-      <c r="A56" s="30">
-        <v>55</v>
-      </c>
-      <c r="B56" s="30">
-        <v>100</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>618</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>617</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>379</v>
-      </c>
-      <c r="F56" s="2" t="s">
-        <v>378</v>
-      </c>
-      <c r="G56" s="30">
-        <v>100</v>
-      </c>
-      <c r="H56" s="30">
-        <v>0</v>
-      </c>
-      <c r="I56" s="2">
-        <v>0.10730000000000001</v>
-      </c>
-      <c r="J56" s="31">
-        <v>10.73</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" s="2" customFormat="1">
-      <c r="A57" s="30">
-        <v>56</v>
-      </c>
-      <c r="B57" s="30">
-        <v>10</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>621</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>620</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>623</v>
-      </c>
-      <c r="F57" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="G57" s="30">
-        <v>10</v>
-      </c>
-      <c r="H57" s="30">
-        <v>0</v>
-      </c>
-      <c r="I57" s="2">
-        <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="J57" s="31">
-        <v>0.17</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" s="2" customFormat="1">
-      <c r="A58" s="30">
-        <v>57</v>
-      </c>
-      <c r="B58" s="30">
-        <v>100</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>639</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>640</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>641</v>
-      </c>
-      <c r="G58" s="30">
-        <v>100</v>
-      </c>
-      <c r="H58" s="30">
-        <v>0</v>
-      </c>
-      <c r="I58" s="2">
-        <v>6.0999999999999999E-2</v>
-      </c>
-      <c r="J58" s="31">
-        <v>6.1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" s="2" customFormat="1">
-      <c r="A59" s="30">
-        <v>58</v>
-      </c>
-      <c r="B59" s="30">
-        <v>20</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>642</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>643</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>644</v>
-      </c>
-      <c r="G59" s="30">
-        <v>20</v>
-      </c>
-      <c r="H59" s="30">
-        <v>0</v>
-      </c>
-      <c r="I59" s="2">
-        <v>0.19400000000000001</v>
-      </c>
-      <c r="J59" s="31">
-        <v>3.88</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" s="2" customFormat="1">
-      <c r="A60" s="30">
-        <v>59</v>
-      </c>
-      <c r="B60" s="30">
-        <v>10</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>645</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>646</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>647</v>
-      </c>
-      <c r="F60" s="2" t="s">
-        <v>648</v>
-      </c>
-      <c r="G60" s="30">
-        <v>10</v>
-      </c>
-      <c r="H60" s="30">
-        <v>0</v>
-      </c>
-      <c r="I60" s="2">
-        <v>0.221</v>
-      </c>
-      <c r="J60" s="31">
-        <v>2.21</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" s="2" customFormat="1">
-      <c r="A61" s="30">
-        <v>60</v>
-      </c>
-      <c r="B61" s="30">
-        <v>1</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>649</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>650</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>651</v>
-      </c>
-      <c r="G61" s="30">
-        <v>1</v>
-      </c>
-      <c r="H61" s="30">
-        <v>0</v>
-      </c>
-      <c r="I61" s="2">
-        <v>16.989999999999998</v>
-      </c>
-      <c r="J61" s="31">
-        <v>16.989999999999998</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" s="2" customFormat="1">
-      <c r="A62" s="30">
-        <v>61</v>
-      </c>
-      <c r="B62" s="30">
-        <v>1</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>652</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>653</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>654</v>
-      </c>
-      <c r="G62" s="30">
-        <v>1</v>
-      </c>
-      <c r="H62" s="30">
-        <v>0</v>
-      </c>
-      <c r="I62" s="2">
-        <v>20.57</v>
-      </c>
-      <c r="J62" s="31">
-        <v>20.57</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" s="2" customFormat="1">
-      <c r="A63" s="30">
-        <v>62</v>
-      </c>
-      <c r="B63" s="30">
-        <v>1</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>655</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>656</v>
-      </c>
-      <c r="E63" s="2" t="s">
-        <v>657</v>
-      </c>
-      <c r="G63" s="30">
-        <v>1</v>
-      </c>
-      <c r="H63" s="30">
-        <v>0</v>
-      </c>
-      <c r="I63" s="2">
-        <v>20.57</v>
-      </c>
-      <c r="J63" s="31">
-        <v>20.57</v>
+      <c r="H64" s="28">
+        <v>0</v>
+      </c>
+      <c r="I64" s="27">
+        <v>0.25900000000000001</v>
+      </c>
+      <c r="J64" s="29">
+        <v>5.18</v>
       </c>
     </row>
   </sheetData>
@@ -4797,8 +4856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2562D6D-91E2-409A-AA1E-33B048E14D93}">
   <dimension ref="A1:X59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -5334,13 +5393,13 @@
       <c r="P8" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="R8" s="12" t="e">
+      <c r="R8" s="12">
         <f>_xlfn.XLOOKUP(D8,cart!$F:$F,cart!$B:$B)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="S8" s="13" t="e">
+        <v>50</v>
+      </c>
+      <c r="S8" s="13">
         <f t="shared" si="1"/>
-        <v>#N/A</v>
+        <v>18</v>
       </c>
       <c r="T8" s="12">
         <f>_xlfn.XLOOKUP(D8,kicad_bom!$F:$F,kicad_bom!$B:$B)</f>
@@ -5468,11 +5527,11 @@
       </c>
       <c r="R10" s="12">
         <f>_xlfn.XLOOKUP(D10,cart!$F:$F,cart!$B:$B)</f>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="S10" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="T10" s="12">
         <f>_xlfn.XLOOKUP(D10,kicad_bom!$F:$F,kicad_bom!$B:$B)</f>
@@ -5534,11 +5593,11 @@
       </c>
       <c r="R11" s="12">
         <f>_xlfn.XLOOKUP(D11,cart!$F:$F,cart!$B:$B)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S11" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T11" s="12">
         <f>_xlfn.XLOOKUP(D11,kicad_bom!$F:$F,kicad_bom!$B:$B)</f>
@@ -6129,11 +6188,11 @@
       </c>
       <c r="R20" s="12">
         <f>_xlfn.XLOOKUP(D20,cart!$F:$F,cart!$B:$B)</f>
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="S20" s="13">
         <f t="shared" si="1"/>
-        <v>-4</v>
+        <v>96</v>
       </c>
       <c r="T20" s="12">
         <f>_xlfn.XLOOKUP(D20,kicad_bom!$F:$F,kicad_bom!$B:$B)</f>
@@ -6393,11 +6452,11 @@
       </c>
       <c r="R24" s="12">
         <f>_xlfn.XLOOKUP(D24,cart!$F:$F,cart!$B:$B)</f>
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="S24" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="T24" s="12">
         <f>_xlfn.XLOOKUP(D24,kicad_bom!$F:$F,kicad_bom!$B:$B)</f>
@@ -6459,11 +6518,11 @@
       </c>
       <c r="R25" s="12">
         <f>_xlfn.XLOOKUP(D25,cart!$F:$F,cart!$B:$B)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S25" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T25" s="12">
         <f>_xlfn.XLOOKUP(D25,kicad_bom!$F:$F,kicad_bom!$B:$B)</f>
@@ -7061,7 +7120,7 @@
         <v>3</v>
       </c>
       <c r="U34" s="13">
-        <f t="shared" ref="U34:U65" si="2">T34-H34</f>
+        <f t="shared" ref="U34:U56" si="2">T34-H34</f>
         <v>0</v>
       </c>
     </row>
@@ -7644,11 +7703,11 @@
       </c>
       <c r="R43" s="12">
         <f>_xlfn.XLOOKUP(D43,cart!$F:$F,cart!$B:$B)</f>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="S43" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="T43" s="12">
         <f>_xlfn.XLOOKUP(D43,kicad_bom!$F:$F,kicad_bom!$B:$B)</f>
@@ -12715,7 +12774,7 @@
         <v>0</v>
       </c>
       <c r="T66" s="5">
-        <f t="shared" ref="T66:T97" si="4">S66-B66</f>
+        <f t="shared" ref="T66:T83" si="4">S66-B66</f>
         <v>-1</v>
       </c>
       <c r="U66" s="12">

</xml_diff>